<commit_message>
fix template for eng
</commit_message>
<xml_diff>
--- a/Template/Piping Template for ENG.xlsx
+++ b/Template/Piping Template for ENG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monitoring Piping\Timas-Monitoring-Piping-V4\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monitoring Piping Fix\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F56AA9-7F3F-4DA0-94FA-7C41C31FD611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70FF844-8A2B-4278-9FDE-4F32B32B899B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="419" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="69">
   <si>
     <t>NS</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>J.05</t>
-  </si>
-  <si>
-    <t>J.01A</t>
   </si>
 </sst>
 </file>
@@ -525,38 +522,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -564,6 +531,12 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -606,8 +579,32 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -632,42 +629,7 @@
     <cellStyle name="Normal 4 2 3" xfId="6" xr:uid="{C770AE6A-C0E2-4DEA-8252-1D92C922AAC0}"/>
     <cellStyle name="Percent 2" xfId="1" xr:uid="{F0E998EA-902E-4628-ABE4-00A5FA70941A}"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -1093,55 +1055,55 @@
       <c r="L1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="42" t="s">
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="42" t="s">
+      <c r="AB1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" s="39" t="s">
+      <c r="AC1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="41"/>
-      <c r="AG1" s="39" t="s">
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="41"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="33"/>
     </row>
     <row r="2" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
@@ -1156,62 +1118,62 @@
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="21" t="s">
+      <c r="M2" s="41"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="U2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="W2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="21" t="s">
+      <c r="X2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="31" t="s">
+      <c r="Y2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="33" t="s">
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="27" t="s">
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AF2" s="37" t="s">
+      <c r="AF2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="35" t="s">
+      <c r="AG2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="27" t="s">
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AJ2" s="37" t="s">
+      <c r="AJ2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AK2" s="29" t="s">
+      <c r="AK2" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="15"/>
-      <c r="C3" s="43"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -1221,43 +1183,43 @@
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="22"/>
-      <c r="X3" s="22"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
       <c r="Y3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="22"/>
-      <c r="AB3" s="22"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
       <c r="AC3" s="8" t="s">
         <v>25</v>
       </c>
       <c r="AD3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="38"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="30"/>
       <c r="AG3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AH3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AI3" s="28"/>
-      <c r="AJ3" s="38"/>
-      <c r="AK3" s="30"/>
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="30"/>
+      <c r="AK3" s="22"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1804,13 +1766,20 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="T1:Z1"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="Q1:Q3"/>
     <mergeCell ref="AI2:AI3"/>
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="AK2:AK3"/>
@@ -1827,53 +1796,46 @@
     <mergeCell ref="AF2:AF3"/>
     <mergeCell ref="AG1:AK1"/>
     <mergeCell ref="AB1:AB3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="T1:Z1"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="M1:M3"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="C1:C3"/>
   </mergeCells>
   <conditionalFormatting sqref="AC5:AK5">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>AND(#REF!&lt;&gt;"", $N9="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:L9">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5:Q5">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:G9 P6:R9 V5:X9">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1884,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DCFF88-2D82-41EE-9D92-2538D2443C73}">
-  <dimension ref="A1:AK9"/>
+  <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,55 +1894,55 @@
       <c r="L1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="42" t="s">
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="42" t="s">
+      <c r="AB1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" s="39" t="s">
+      <c r="AC1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="41"/>
-      <c r="AG1" s="39" t="s">
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="41"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="33"/>
     </row>
     <row r="2" spans="1:37" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
@@ -1995,55 +1957,55 @@
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="21" t="s">
+      <c r="M2" s="41"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="U2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="W2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="21" t="s">
+      <c r="X2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="31" t="s">
+      <c r="Y2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="33" t="s">
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="27" t="s">
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AF2" s="37" t="s">
+      <c r="AF2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="35" t="s">
+      <c r="AG2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="27" t="s">
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AJ2" s="37" t="s">
+      <c r="AJ2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AK2" s="29" t="s">
+      <c r="AK2" s="21" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2060,43 +2022,43 @@
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="22"/>
-      <c r="X3" s="22"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
       <c r="Y3" s="11" t="s">
         <v>25</v>
       </c>
       <c r="Z3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="22"/>
-      <c r="AB3" s="22"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
       <c r="AC3" s="12" t="s">
         <v>25</v>
       </c>
       <c r="AD3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="38"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="30"/>
       <c r="AG3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AH3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AI3" s="28"/>
-      <c r="AJ3" s="38"/>
-      <c r="AK3" s="30"/>
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="30"/>
+      <c r="AK3" s="22"/>
     </row>
     <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -2212,88 +2174,13 @@
       </c>
     </row>
     <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>45738</v>
-      </c>
-      <c r="B5" s="13">
-        <v>45738</v>
-      </c>
-      <c r="C5" s="13">
-        <v>45738</v>
-      </c>
-      <c r="D5" s="13">
-        <v>45738</v>
-      </c>
-      <c r="E5" s="13">
-        <v>45738</v>
-      </c>
-      <c r="F5" s="13">
-        <v>45738</v>
-      </c>
-      <c r="G5" s="13">
-        <v>45738</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <v>851</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="S5" s="1">
-        <v>3</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="X5" s="1">
-        <v>15</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="AA5" s="1">
-        <f t="shared" ref="AA5:AA9" si="0">Y5+Z5</f>
-        <v>0.5</v>
-      </c>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
       <c r="AE5" s="13"/>
       <c r="AI5" s="13"/>
     </row>
@@ -2330,38 +2217,14 @@
       <c r="AE8" s="13"/>
       <c r="AI8" s="13"/>
     </row>
-    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AI9" s="13"/>
-    </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="T1:Z1"/>
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="AB1:AB3"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG1:AK1"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
@@ -2374,46 +2237,44 @@
     <mergeCell ref="O1:O3"/>
     <mergeCell ref="P1:P3"/>
     <mergeCell ref="Q1:Q3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="AG1:AK1"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="T1:Z1"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="AB1:AB3"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
   </mergeCells>
-  <conditionalFormatting sqref="AC5:AK5">
-    <cfRule type="expression" dxfId="13" priority="6">
+  <conditionalFormatting sqref="H5 H7 J5:L8">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB5">
-    <cfRule type="expression" dxfId="12" priority="7">
-      <formula>AND(#REF!&lt;&gt;"", $N9="")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6 H8 J5:L9">
-    <cfRule type="expression" dxfId="11" priority="5">
+  <conditionalFormatting sqref="A5:G8 V5:X8">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P5:Q5">
-    <cfRule type="expression" dxfId="10" priority="4">
+  <conditionalFormatting sqref="H6 P5:R8">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R5">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:G9 H7 P6:R9 V5:X9">
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5 H9">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>AND(#REF!&lt;&gt;"", $N5="")</formula>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(#REF!&lt;&gt;"", $N8="")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>